<commit_message>
Employement details script updated
</commit_message>
<xml_diff>
--- a/Data/Result/ResEmployee.xlsx
+++ b/Data/Result/ResEmployee.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="12">
   <si>
     <t>TestId</t>
   </si>
@@ -1105,7 +1105,7 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Leave muster implementation started
</commit_message>
<xml_diff>
--- a/Data/Result/ResEmployee.xlsx
+++ b/Data/Result/ResEmployee.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="20">
   <si>
     <t>TestId</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>editemp_007</t>
+  </si>
+  <si>
+    <t>E</t>
   </si>
 </sst>
 </file>
@@ -1126,7 +1129,7 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Employee Photo and Document Uploading completed
</commit_message>
<xml_diff>
--- a/Data/Result/ResEmployee.xlsx
+++ b/Data/Result/ResEmployee.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>TestId</t>
   </si>
@@ -1068,7 +1068,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -1079,7 +1079,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
@@ -1090,7 +1090,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
Implemented Calculation of execition time
</commit_message>
<xml_diff>
--- a/Data/Result/ResEmployee.xlsx
+++ b/Data/Result/ResEmployee.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="23">
   <si>
     <t>TestId</t>
   </si>
@@ -1068,7 +1068,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
@@ -1079,7 +1079,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
@@ -1090,7 +1090,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D4" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Employee Creation module updated with Dale selection implementation
</commit_message>
<xml_diff>
--- a/Data/Result/ResEmployee.xlsx
+++ b/Data/Result/ResEmployee.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="24">
   <si>
     <t>TestId</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>597112896692,00002</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -1068,7 +1071,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>

</xml_diff>